<commit_message>
this experimentts conclude investigation of inventories and WSD approach for the moment
</commit_message>
<xml_diff>
--- a/experiment/Results.xlsx
+++ b/experiment/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>All experiments are based on vectors trained on english Wikipedia (12 GB)</t>
   </si>
@@ -93,7 +93,10 @@
     <t>weighted</t>
   </si>
   <si>
-    <t>double check stanford results!</t>
+    <t>weighted + average context</t>
+  </si>
+  <si>
+    <t>weighted + avg + cosine</t>
   </si>
 </sst>
 </file>
@@ -264,8 +267,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -301,7 +310,7 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -309,6 +318,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -316,9 +328,176 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -498,8 +677,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:D16" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="Column1" headerRowDxfId="8" dataDxfId="7"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="6"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="14" dataDxfId="13"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="12"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
   </tableColumns>
@@ -508,16 +687,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A21:H29" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="8">
-    <tableColumn id="1" name="Column1" headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A21:M29" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="13">
+    <tableColumn id="1" name="Column1" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="9"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5" dataDxfId="2"/>
-    <tableColumn id="6" name="Column6" dataDxfId="1"/>
-    <tableColumn id="7" name="Column7" dataDxfId="0"/>
-    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="5" name="Column5" dataDxfId="8"/>
+    <tableColumn id="6" name="Column6" dataDxfId="7"/>
+    <tableColumn id="7" name="Column7" dataDxfId="6"/>
+    <tableColumn id="8" name="Column8" dataDxfId="5"/>
+    <tableColumn id="9" name="Column9" dataDxfId="4"/>
+    <tableColumn id="10" name="Column10" dataDxfId="3"/>
+    <tableColumn id="11" name="Column11" dataDxfId="2"/>
+    <tableColumn id="12" name="Column12" dataDxfId="1"/>
+    <tableColumn id="13" name="Column13" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -845,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1002,23 +1186,31 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:13">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:13">
       <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -1030,8 +1222,18 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="6"/>
       <c r="B22" s="3" t="s">
         <v>18</v>
@@ -1051,8 +1253,26 @@
       <c r="G22" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="H22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="7" t="s">
         <v>7</v>
       </c>
@@ -1065,22 +1285,52 @@
       <c r="D23" s="13">
         <v>0.38299943222999999</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="E23" s="12">
+        <v>0.38708630759200002</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.38702351987</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.38705491118500002</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0.38708630759200002</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0.38702351987</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0.38705491118500002</v>
+      </c>
+      <c r="K23" s="12"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="B24" s="11">
+        <v>0.35999351070699998</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.35993511759899999</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.35996431178499999</v>
+      </c>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
@@ -1096,11 +1346,14 @@
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="H25" s="12"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
@@ -1116,8 +1369,14 @@
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
@@ -1133,8 +1392,14 @@
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
@@ -1156,8 +1421,26 @@
       <c r="G28" s="15">
         <v>0.52130854777199997</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="H28" s="14">
+        <v>0.52209944751399995</v>
+      </c>
+      <c r="I28" s="15">
+        <v>0.52116788321200003</v>
+      </c>
+      <c r="J28" s="15">
+        <v>0.52163324945199996</v>
+      </c>
+      <c r="K28" s="14">
+        <v>0.52209944751399995</v>
+      </c>
+      <c r="L28" s="15">
+        <v>0.52116788321200003</v>
+      </c>
+      <c r="M28" s="15">
+        <v>0.52163324945199996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="7" t="s">
         <v>14</v>
       </c>
@@ -1167,9 +1450,16 @@
       <c r="E29" s="16"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Experiments on full TWSI
</commit_message>
<xml_diff>
--- a/experiment/Results.xlsx
+++ b/experiment/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
   <si>
     <t>All experiments are based on vectors trained on english Wikipedia (12 GB)</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Most frequent sense (TWSI dev set)</t>
+  </si>
+  <si>
+    <t>Evaluation (TWSI full set)</t>
+  </si>
+  <si>
+    <t>Upper bound (TWSI full set)</t>
+  </si>
+  <si>
+    <t>Most frequent sense (TWSI full set)</t>
   </si>
 </sst>
 </file>
@@ -113,7 +122,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +169,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -181,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -300,8 +315,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -331,8 +377,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -343,7 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -364,10 +415,36 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -382,6 +459,9 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -396,9 +476,12 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
     <dxf>
       <font>
         <b val="0"/>
@@ -422,6 +505,14 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -470,6 +561,30 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -870,18 +985,6 @@
       </font>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -904,10 +1007,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:G16" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:G16" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="5">
   <tableColumns count="7">
-    <tableColumn id="1" name="Column1" headerRowDxfId="20" dataDxfId="19"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="18"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="22" dataDxfId="4"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="21" dataDxfId="3"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
     <tableColumn id="5" name="Column5" dataDxfId="2"/>
@@ -919,24 +1022,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A21:P29" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A21:P30" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="16">
-    <tableColumn id="1" name="Column1" headerRowDxfId="17" dataDxfId="16"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="15"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="20" dataDxfId="19"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="18"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5" dataDxfId="14"/>
-    <tableColumn id="6" name="Column6" dataDxfId="13"/>
-    <tableColumn id="7" name="Column7" dataDxfId="12"/>
-    <tableColumn id="8" name="Column8" dataDxfId="11"/>
-    <tableColumn id="9" name="Column9" dataDxfId="10"/>
-    <tableColumn id="10" name="Column10" dataDxfId="9"/>
-    <tableColumn id="11" name="Column11" dataDxfId="8"/>
-    <tableColumn id="12" name="Column12" dataDxfId="7"/>
-    <tableColumn id="13" name="Column13" dataDxfId="6"/>
-    <tableColumn id="14" name="Column14" dataDxfId="5"/>
-    <tableColumn id="15" name="Column15" dataDxfId="4"/>
-    <tableColumn id="16" name="Column16" dataDxfId="3"/>
+    <tableColumn id="5" name="Column5" dataDxfId="17"/>
+    <tableColumn id="6" name="Column6" dataDxfId="16"/>
+    <tableColumn id="7" name="Column7" dataDxfId="15"/>
+    <tableColumn id="8" name="Column8" dataDxfId="14"/>
+    <tableColumn id="9" name="Column9" dataDxfId="13"/>
+    <tableColumn id="10" name="Column10" dataDxfId="12"/>
+    <tableColumn id="11" name="Column11" dataDxfId="11"/>
+    <tableColumn id="12" name="Column12" dataDxfId="10"/>
+    <tableColumn id="13" name="Column13" dataDxfId="9"/>
+    <tableColumn id="14" name="Column14" dataDxfId="8"/>
+    <tableColumn id="15" name="Column15" dataDxfId="7"/>
+    <tableColumn id="16" name="Column16" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1276,17 +1379,17 @@
     <col min="3" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1303,28 +1406,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:14">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8" s="39"/>
+      <c r="G8" s="41"/>
+      <c r="I8" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="39"/>
+      <c r="N8" s="41"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="6"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="54" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1339,134 +1454,212 @@
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="42" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="55">
         <v>1</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="51">
         <v>0.48807785888100003</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="51">
         <v>0.65598430346600001</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>0.37032824179399998</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <v>0.36966747769699998</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="44">
         <v>0.36999756473700002</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I10" s="43">
+        <v>1</v>
+      </c>
+      <c r="J10" s="29">
+        <v>0.75121951219500005</v>
+      </c>
+      <c r="K10" s="29">
+        <v>0.85793871866299998</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0.67662989105299998</v>
+      </c>
+      <c r="M10" s="29">
+        <v>0.67566487529300001</v>
+      </c>
+      <c r="N10" s="44">
+        <v>0.67614703884899996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="55">
         <v>1</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="51">
         <v>0.52635847526400004</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="51">
         <v>0.68969181721600004</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
+      <c r="I11" s="45">
+        <v>1</v>
+      </c>
+      <c r="J11" s="46">
+        <v>0.77315006200900005</v>
+      </c>
+      <c r="K11" s="46">
+        <v>0.87206388063200002</v>
+      </c>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="55">
         <v>1</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="51">
         <v>0.724249797242</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="51">
         <v>0.84007525870199995</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="44"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="44"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="55">
         <v>1</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="51">
         <v>0.67072181670700004</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="51">
         <v>0.80291262135899999</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="47"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="55">
         <v>1</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="51">
         <v>0.59772911597699996</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="51">
         <v>0.748223350254</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="44"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="44"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="55">
         <v>1</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="51">
         <v>0.99821573398200003</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="51">
         <v>0.99910707037900004</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="46">
         <v>0.37536561586</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="46">
         <v>0.37469586374699998</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="47">
         <v>0.37503044078300002</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="I15" s="45"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="47"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="50"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
@@ -1518,11 +1711,11 @@
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="19" t="s">
+      <c r="N21" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="24"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="23"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="6"/>
@@ -1562,13 +1755,13 @@
       <c r="M22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="N22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="O22" s="21" t="s">
+      <c r="O22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="P22" s="25" t="s">
+      <c r="P22" s="24" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1576,43 +1769,43 @@
       <c r="A23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <v>0.383030499676</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="12">
         <v>0.38296836982999999</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="12">
         <v>0.38299943222999999</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="11">
         <v>0.38708630759200002</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <v>0.38702351987</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <v>0.38705491118500002</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <v>0.38708630759200002</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="12">
         <v>0.38702351987</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="12">
         <v>0.38705491118500002</v>
       </c>
-      <c r="K23" s="12"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="12">
+      <c r="K23" s="11"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="11">
         <v>0.38270603504200001</v>
       </c>
-      <c r="O23" s="13">
+      <c r="O23" s="12">
         <v>0.38264395782600003</v>
       </c>
-      <c r="P23" s="26">
+      <c r="P23" s="25">
         <v>0.38267499391699999</v>
       </c>
     </row>
@@ -1620,153 +1813,153 @@
       <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>0.35999351070699998</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>0.35993511759899999</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <v>0.35996431178499999</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="27"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>0.27526811829699999</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>0.27477696674800001</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="10">
         <v>0.27502232324100001</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="26"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="25"/>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <v>0.30500487487</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>0.30446066504500002</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>0.30473252699100001</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="27"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="26"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="10">
         <v>0.33782905427400001</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>0.33722627737200001</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="10">
         <v>0.337527396704</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="26"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="25"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="10">
         <v>0.484075398115</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="10">
         <v>0.483211678832</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="10">
         <v>0.48364315285300002</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="13">
         <v>0.52177445563900005</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="14">
         <v>0.52084347120800001</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="14">
         <v>0.52130854777199997</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="13">
         <v>0.52209944751399995</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="14">
         <v>0.52116788321200003</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="14">
         <v>0.52163324945199996</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28" s="13">
         <v>0.52209944751399995</v>
       </c>
-      <c r="L28" s="15">
+      <c r="L28" s="14">
         <v>0.52116788321200003</v>
       </c>
-      <c r="M28" s="15">
+      <c r="M28" s="14">
         <v>0.52163324945199996</v>
       </c>
-      <c r="N28" s="22">
+      <c r="N28" s="21">
         <v>0.51153721156999998</v>
       </c>
-      <c r="O28" s="23">
+      <c r="O28" s="22">
         <v>0.510624493106</v>
       </c>
-      <c r="P28" s="27">
+      <c r="P28" s="26">
         <v>0.51108044484100001</v>
       </c>
     </row>
@@ -1774,21 +1967,152 @@
       <c r="A29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="28"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="27"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="7"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="37"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="31"/>
+      <c r="B32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0.64556299057900002</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0.64542510679300003</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.64549404132300003</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0.65718873398599997</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.65704836709400005</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0.65711854304399997</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0.65727143044199998</v>
+      </c>
+      <c r="I33" s="12">
+        <v>0.657131045887</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0.65720123066699998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="34">
+        <v>0.57668373429599995</v>
+      </c>
+      <c r="C34" s="34">
+        <v>0.57656056221600005</v>
+      </c>
+      <c r="D34" s="34">
+        <v>0.57662214167799997</v>
+      </c>
+      <c r="E34" s="13">
+        <v>0.59163111867600005</v>
+      </c>
+      <c r="F34" s="14">
+        <v>0.591504754031</v>
+      </c>
+      <c r="G34" s="14">
+        <v>0.59156792960500004</v>
+      </c>
+      <c r="H34" s="13">
+        <v>0.59170003238900004</v>
+      </c>
+      <c r="I34" s="14">
+        <v>0.59157365302499998</v>
+      </c>
+      <c r="J34" s="14">
+        <v>0.59163683595799998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Evaluation of sim WSD approach
</commit_message>
<xml_diff>
--- a/experiment/Results.xlsx
+++ b/experiment/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
   <si>
     <t>All experiments are based on vectors trained on english Wikipedia (12 GB)</t>
   </si>
@@ -347,8 +347,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,7 +448,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -462,6 +466,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -479,113 +485,11 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -969,7 +873,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -979,10 +883,83 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1001,21 +978,52 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:G16" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:G16" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="22">
   <tableColumns count="7">
-    <tableColumn id="1" name="Column1" headerRowDxfId="22" dataDxfId="4"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="21" dataDxfId="3"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="19" dataDxfId="18"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5" dataDxfId="2"/>
-    <tableColumn id="6" name="Column6" dataDxfId="1"/>
-    <tableColumn id="7" name="Column7" dataDxfId="0"/>
+    <tableColumn id="5" name="Column5" dataDxfId="17"/>
+    <tableColumn id="6" name="Column6" dataDxfId="16"/>
+    <tableColumn id="7" name="Column7" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1024,22 +1032,22 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A21:P30" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="16">
-    <tableColumn id="1" name="Column1" headerRowDxfId="20" dataDxfId="19"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="18"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="14" dataDxfId="13"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="12"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5" dataDxfId="17"/>
-    <tableColumn id="6" name="Column6" dataDxfId="16"/>
-    <tableColumn id="7" name="Column7" dataDxfId="15"/>
-    <tableColumn id="8" name="Column8" dataDxfId="14"/>
-    <tableColumn id="9" name="Column9" dataDxfId="13"/>
-    <tableColumn id="10" name="Column10" dataDxfId="12"/>
-    <tableColumn id="11" name="Column11" dataDxfId="11"/>
-    <tableColumn id="12" name="Column12" dataDxfId="10"/>
-    <tableColumn id="13" name="Column13" dataDxfId="9"/>
-    <tableColumn id="14" name="Column14" dataDxfId="8"/>
-    <tableColumn id="15" name="Column15" dataDxfId="7"/>
-    <tableColumn id="16" name="Column16" dataDxfId="6"/>
+    <tableColumn id="5" name="Column5" dataDxfId="11"/>
+    <tableColumn id="6" name="Column6" dataDxfId="10"/>
+    <tableColumn id="7" name="Column7" dataDxfId="9"/>
+    <tableColumn id="8" name="Column8" dataDxfId="8"/>
+    <tableColumn id="9" name="Column9" dataDxfId="7"/>
+    <tableColumn id="10" name="Column10" dataDxfId="6"/>
+    <tableColumn id="11" name="Column11" dataDxfId="5"/>
+    <tableColumn id="12" name="Column12" dataDxfId="4"/>
+    <tableColumn id="13" name="Column13" dataDxfId="3"/>
+    <tableColumn id="14" name="Column14" dataDxfId="2"/>
+    <tableColumn id="15" name="Column15" dataDxfId="1"/>
+    <tableColumn id="16" name="Column16" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1370,7 +1378,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1796,9 +1804,15 @@
       <c r="J23" s="12">
         <v>0.38705491118500002</v>
       </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+      <c r="K23" s="11">
+        <v>0.39746917586000002</v>
+      </c>
+      <c r="L23" s="12">
+        <v>0.39740470397400002</v>
+      </c>
+      <c r="M23" s="12">
+        <v>0.39743693730200003</v>
+      </c>
       <c r="N23" s="11">
         <v>0.38270603504200001</v>
       </c>
@@ -1945,13 +1959,13 @@
         <v>0.52163324945199996</v>
       </c>
       <c r="K28" s="13">
-        <v>0.52209944751399995</v>
+        <v>0.53282417939600002</v>
       </c>
       <c r="L28" s="14">
-        <v>0.52116788321200003</v>
+        <v>0.53187347931899998</v>
       </c>
       <c r="M28" s="14">
-        <v>0.52163324945199996</v>
+        <v>0.53234840490299995</v>
       </c>
       <c r="N28" s="21">
         <v>0.51153721156999998</v>
@@ -1999,6 +2013,9 @@
         <v>24</v>
       </c>
       <c r="J30" s="37"/>
+      <c r="L30" s="37" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="30" t="s">
@@ -2019,6 +2036,11 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
+      <c r="K31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="31"/>
@@ -2049,8 +2071,17 @@
       <c r="J32" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="32" t="s">
         <v>7</v>
       </c>
@@ -2081,8 +2112,17 @@
       <c r="J33" s="12">
         <v>0.65720123066699998</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <v>0.66928998201400003</v>
+      </c>
+      <c r="L33">
+        <v>0.66914703045299995</v>
+      </c>
+      <c r="M33">
+        <v>0.66921849859899996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="33" t="s">
         <v>8</v>
       </c>
@@ -2112,6 +2152,15 @@
       </c>
       <c r="J34" s="14">
         <v>0.59163683595799998</v>
+      </c>
+      <c r="K34">
+        <v>0.62832077955200005</v>
+      </c>
+      <c r="L34">
+        <v>0.62818657847600001</v>
+      </c>
+      <c r="M34">
+        <v>0.62825367184699998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added evaluation on induced sense vectors (clustering of neighbours, without frequency weighting)
</commit_message>
<xml_diff>
--- a/experiment/Results.xlsx
+++ b/experiment/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="43">
   <si>
     <t>All experiments are based on vectors trained on english Wikipedia (12 GB)</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Vectors:</t>
   </si>
   <si>
-    <t>induced</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>weighted + avg + cosine</t>
   </si>
   <si>
-    <t>weighted + avg + filter ctx</t>
-  </si>
-  <si>
     <t>Most frequent sense (TWSI dev set)</t>
   </si>
   <si>
@@ -112,6 +106,48 @@
   </si>
   <si>
     <t>Most frequent sense (TWSI full set)</t>
+  </si>
+  <si>
+    <t>Context filtering investigation:</t>
+  </si>
+  <si>
+    <t>weighted + avg + filter multisense words</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>twsi inventory</t>
+  </si>
+  <si>
+    <t>wiki inventory</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>filter5</t>
+  </si>
+  <si>
+    <t>filter3</t>
+  </si>
+  <si>
+    <t>filter1</t>
+  </si>
+  <si>
+    <t>take N most informative context words</t>
+  </si>
+  <si>
+    <t>filter2</t>
+  </si>
+  <si>
+    <t>custom100</t>
+  </si>
+  <si>
+    <t>custom70</t>
+  </si>
+  <si>
+    <t>weighted + avg +cosine + best filter (2)</t>
   </si>
 </sst>
 </file>
@@ -207,15 +243,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -283,17 +310,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -302,17 +318,6 @@
         <color theme="4"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -346,8 +351,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,68 +429,123 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -468,6 +565,25 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -487,6 +603,25 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
@@ -1015,7 +1150,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:G16" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:G17" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="22">
   <tableColumns count="7">
     <tableColumn id="1" name="Column1" headerRowDxfId="21" dataDxfId="20"/>
     <tableColumn id="2" name="Column2" headerRowDxfId="19" dataDxfId="18"/>
@@ -1030,7 +1165,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A21:P30" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A22:P34" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="16">
     <tableColumn id="1" name="Column1" headerRowDxfId="14" dataDxfId="13"/>
     <tableColumn id="2" name="Column2" headerRowDxfId="12"/>
@@ -1375,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1422,106 +1557,106 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="38"/>
+      <c r="I8" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="41"/>
-      <c r="I8" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="39"/>
-      <c r="N8" s="41"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="36"/>
+      <c r="N8" s="38"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="6"/>
-      <c r="B9" s="54" t="s">
-        <v>18</v>
+      <c r="B9" s="48" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="J9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="42" t="s">
-        <v>16</v>
+      <c r="N9" s="39" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="49">
         <v>1</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="45">
         <v>0.48807785888100003</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="45">
         <v>0.65598430346600001</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="26">
         <v>0.37032824179399998</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="26">
         <v>0.36966747769699998</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="41">
         <v>0.36999756473700002</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="40">
         <v>1</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="26">
         <v>0.75121951219500005</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="26">
         <v>0.85793871866299998</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="26">
         <v>0.67662989105299998</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="26">
         <v>0.67566487529300001</v>
       </c>
-      <c r="N10" s="44">
+      <c r="N10" s="41">
         <v>0.67614703884899996</v>
       </c>
     </row>
@@ -1529,638 +1664,1014 @@
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="49">
         <v>1</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="45">
         <v>0.52635847526400004</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="45">
         <v>0.68969181721600004</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
-      <c r="I11" s="45">
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+      <c r="I11" s="42">
         <v>1</v>
       </c>
-      <c r="J11" s="46">
+      <c r="J11" s="43">
         <v>0.77315006200900005</v>
       </c>
-      <c r="K11" s="46">
+      <c r="K11" s="43">
         <v>0.87206388063200002</v>
       </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="47"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="55">
+      <c r="B12" s="49">
         <v>1</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="45">
         <v>0.724249797242</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="45">
         <v>0.84007525870199995</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="44"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="44"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="41"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="41"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="55">
+      <c r="B13" s="49">
         <v>1</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="45">
         <v>0.67072181670700004</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="45">
         <v>0.80291262135899999</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="47"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="47"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14" s="49">
         <v>1</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="45">
         <v>0.59772911597699996</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="45">
         <v>0.748223350254</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="44"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="44"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="41"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="55">
+      <c r="B15" s="49">
         <v>1</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="45">
         <v>0.99821573398200003</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="45">
         <v>0.99910707037900004</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="43">
         <v>0.37536561586</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="43">
         <v>0.37469586374699998</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="44">
         <v>0.37503044078300002</v>
       </c>
-      <c r="I15" s="45"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="47"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="49">
+        <v>1</v>
+      </c>
+      <c r="C16" s="45">
+        <v>0.47688564476899997</v>
+      </c>
+      <c r="D16" s="45">
+        <v>0.64579901153200003</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="41"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="41"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="50">
+        <v>1</v>
+      </c>
+      <c r="C17" s="51">
+        <v>0.47931873479300002</v>
+      </c>
+      <c r="D17" s="51">
+        <v>0.64802631578900005</v>
+      </c>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="68"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="67"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="O21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="R21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="D20" s="1" t="s">
+      <c r="E22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22" s="15"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="15"/>
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="6"/>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="P23" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="S23" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0.383030499676</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0.38296836982999999</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.38299943222999999</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0.38708630759200002</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.38702351987</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0.38705491118500002</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0.38708630759200002</v>
+      </c>
+      <c r="I24" s="12">
+        <v>0.38702351987</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0.38705491118500002</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0.39746917586000002</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0.39740470397400002</v>
+      </c>
+      <c r="M24" s="12">
+        <v>0.39743693730200003</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0.40979883192700001</v>
+      </c>
+      <c r="O24" s="14">
+        <v>0.40973236009699998</v>
+      </c>
+      <c r="P24" s="52">
+        <v>0.40976559331700002</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>0.38270603504200001</v>
+      </c>
+      <c r="R24" s="12">
+        <v>0.38264395782600003</v>
+      </c>
+      <c r="S24" s="23">
+        <v>0.38267499391699999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0.35999351070699998</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.35993511759899999</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.35996431178499999</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="24"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.27526811829699999</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.27477696674800001</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.27502232324100001</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="23"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0.30500487487</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0.30446066504500002</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0.30473252699100001</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="24"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0.33782905427400001</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0.33722627737200001</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.337527396704</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="23"/>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0.484075398115</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0.483211678832</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0.48364315285300002</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.52177445563900005</v>
+      </c>
+      <c r="F29" s="14">
+        <v>0.52084347120800001</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0.52130854777199997</v>
+      </c>
+      <c r="H29" s="13">
+        <v>0.52209944751399995</v>
+      </c>
+      <c r="I29" s="14">
+        <v>0.52116788321200003</v>
+      </c>
+      <c r="J29" s="14">
+        <v>0.52163324945199996</v>
+      </c>
+      <c r="K29" s="13">
+        <v>0.53282417939600002</v>
+      </c>
+      <c r="L29" s="14">
+        <v>0.53187347931899998</v>
+      </c>
+      <c r="M29" s="14">
+        <v>0.53234840490299995</v>
+      </c>
+      <c r="N29" s="13">
+        <v>0.58271043223899999</v>
+      </c>
+      <c r="O29" s="10">
+        <v>0.58167072181699997</v>
+      </c>
+      <c r="P29" s="52">
+        <v>0.58219011283400002</v>
+      </c>
+      <c r="Q29" s="19">
+        <v>0.51153721156999998</v>
+      </c>
+      <c r="R29" s="20">
+        <v>0.510624493106</v>
+      </c>
+      <c r="S29" s="24">
+        <v>0.51108044484100001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="K30" s="72">
+        <v>0.38154046148800003</v>
+      </c>
+      <c r="L30" s="10">
+        <v>0.38085969180899998</v>
+      </c>
+      <c r="M30" s="10">
+        <v>0.38119977270900002</v>
+      </c>
+      <c r="N30" s="72">
+        <v>0.39194020149499997</v>
+      </c>
+      <c r="O30" s="10">
+        <v>0.39124087591200002</v>
+      </c>
+      <c r="P30" s="10">
+        <v>0.39159022647899999</v>
+      </c>
+      <c r="Q30" s="64"/>
+      <c r="S30" s="7"/>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="48"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="70">
+        <v>0.383002924927</v>
+      </c>
+      <c r="L31" s="71">
+        <v>0.38231954582299998</v>
+      </c>
+      <c r="M31" s="71">
+        <v>0.38266093026999998</v>
+      </c>
+      <c r="N31" s="17">
+        <v>0.38982775430599997</v>
+      </c>
+      <c r="O31" s="73">
+        <v>0.38913219789100001</v>
+      </c>
+      <c r="P31" s="74">
+        <v>0.38947966555699998</v>
+      </c>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="B32" s="69"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="7"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H34" s="34"/>
+      <c r="I34" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J34" s="34"/>
+      <c r="L34" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="L20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="O20" s="1" t="s">
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="5" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="28"/>
+      <c r="B36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="23"/>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="6"/>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="E36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="F36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="G36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="4" t="s">
+      <c r="J36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="L36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="4" t="s">
+      <c r="M36" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="11">
+        <v>0.64556299057900002</v>
+      </c>
+      <c r="C37" s="12">
+        <v>0.64542510679300003</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0.64549404132300003</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0.65718873398599997</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.65704836709400005</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0.65711854304399997</v>
+      </c>
+      <c r="H37" s="11">
+        <v>0.65727143044199998</v>
+      </c>
+      <c r="I37" s="12">
+        <v>0.657131045887</v>
+      </c>
+      <c r="J37" s="12">
+        <v>0.65720123066699998</v>
+      </c>
+      <c r="K37" s="11">
+        <v>0.66928998201400003</v>
+      </c>
+      <c r="L37" s="11">
+        <v>0.66914703045299995</v>
+      </c>
+      <c r="M37" s="11">
+        <v>0.66921849859899996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="31">
+        <v>0.57668373429599995</v>
+      </c>
+      <c r="C38" s="31">
+        <v>0.57656056221600005</v>
+      </c>
+      <c r="D38" s="31">
+        <v>0.57662214167799997</v>
+      </c>
+      <c r="E38" s="13">
+        <v>0.59163111867600005</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.591504754031</v>
+      </c>
+      <c r="G38" s="14">
+        <v>0.59156792960500004</v>
+      </c>
+      <c r="H38" s="13">
+        <v>0.59170003238900004</v>
+      </c>
+      <c r="I38" s="14">
+        <v>0.59157365302499998</v>
+      </c>
+      <c r="J38" s="14">
+        <v>0.59163683595799998</v>
+      </c>
+      <c r="K38" s="13">
+        <v>0.62832077955200005</v>
+      </c>
+      <c r="L38" s="13">
+        <v>0.62818657847600001</v>
+      </c>
+      <c r="M38" s="13">
+        <v>0.62825367184699998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="C42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="36"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="38"/>
+      <c r="K43" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="L43" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M43" s="36"/>
+      <c r="N43" s="38"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="57"/>
+      <c r="B44" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N22" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="O22" s="20" t="s">
+      <c r="D44" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P22" s="24" t="s">
+      <c r="F44" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="11">
-        <v>0.383030499676</v>
-      </c>
-      <c r="C23" s="12">
-        <v>0.38296836982999999</v>
-      </c>
-      <c r="D23" s="12">
-        <v>0.38299943222999999</v>
-      </c>
-      <c r="E23" s="11">
-        <v>0.38708630759200002</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0.38702351987</v>
-      </c>
-      <c r="G23" s="12">
-        <v>0.38705491118500002</v>
-      </c>
-      <c r="H23" s="11">
-        <v>0.38708630759200002</v>
-      </c>
-      <c r="I23" s="12">
-        <v>0.38702351987</v>
-      </c>
-      <c r="J23" s="12">
-        <v>0.38705491118500002</v>
-      </c>
-      <c r="K23" s="11">
+      <c r="G44" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" s="57"/>
+      <c r="L44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N44" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="62">
+        <v>0.53282417939600002</v>
+      </c>
+      <c r="C45" s="63">
+        <v>0.53187347931899998</v>
+      </c>
+      <c r="D45" s="61">
+        <v>0.53234840490299995</v>
+      </c>
+      <c r="E45" s="11">
         <v>0.39746917586000002</v>
       </c>
-      <c r="L23" s="12">
+      <c r="F45" s="12">
         <v>0.39740470397400002</v>
       </c>
-      <c r="M23" s="12">
+      <c r="G45" s="61">
         <v>0.39743693730200003</v>
       </c>
-      <c r="N23" s="11">
-        <v>0.38270603504200001</v>
-      </c>
-      <c r="O23" s="12">
-        <v>0.38264395782600003</v>
-      </c>
-      <c r="P23" s="25">
-        <v>0.38267499391699999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="10">
-        <v>0.35999351070699998</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0.35993511759899999</v>
-      </c>
-      <c r="D24" s="10">
-        <v>0.35996431178499999</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="26"/>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="10">
-        <v>0.27526811829699999</v>
-      </c>
-      <c r="C25" s="10">
-        <v>0.27477696674800001</v>
-      </c>
-      <c r="D25" s="10">
-        <v>0.27502232324100001</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="25"/>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="10">
-        <v>0.30500487487</v>
-      </c>
-      <c r="C26" s="10">
-        <v>0.30446066504500002</v>
-      </c>
-      <c r="D26" s="10">
-        <v>0.30473252699100001</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="26"/>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="10">
-        <v>0.33782905427400001</v>
-      </c>
-      <c r="C27" s="10">
-        <v>0.33722627737200001</v>
-      </c>
-      <c r="D27" s="10">
-        <v>0.337527396704</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="25"/>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="10">
-        <v>0.484075398115</v>
-      </c>
-      <c r="C28" s="10">
-        <v>0.483211678832</v>
-      </c>
-      <c r="D28" s="10">
-        <v>0.48364315285300002</v>
-      </c>
-      <c r="E28" s="13">
-        <v>0.52177445563900005</v>
-      </c>
-      <c r="F28" s="14">
-        <v>0.52084347120800001</v>
-      </c>
-      <c r="G28" s="14">
-        <v>0.52130854777199997</v>
-      </c>
-      <c r="H28" s="13">
-        <v>0.52209944751399995</v>
-      </c>
-      <c r="I28" s="14">
-        <v>0.52116788321200003</v>
-      </c>
-      <c r="J28" s="14">
-        <v>0.52163324945199996</v>
-      </c>
-      <c r="K28" s="13">
-        <v>0.53282417939600002</v>
-      </c>
-      <c r="L28" s="14">
-        <v>0.53187347931899998</v>
-      </c>
-      <c r="M28" s="14">
-        <v>0.53234840490299995</v>
-      </c>
-      <c r="N28" s="21">
-        <v>0.51153721156999998</v>
-      </c>
-      <c r="O28" s="22">
-        <v>0.510624493106</v>
-      </c>
-      <c r="P28" s="26">
-        <v>0.51108044484100001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="27"/>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="7"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37" t="s">
+      <c r="H45" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="37"/>
-      <c r="L30" s="37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="31"/>
-      <c r="B32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M32" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="11">
-        <v>0.64556299057900002</v>
-      </c>
-      <c r="C33" s="12">
-        <v>0.64542510679300003</v>
-      </c>
-      <c r="D33" s="12">
-        <v>0.64549404132300003</v>
-      </c>
-      <c r="E33" s="11">
-        <v>0.65718873398599997</v>
-      </c>
-      <c r="F33" s="12">
-        <v>0.65704836709400005</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0.65711854304399997</v>
-      </c>
-      <c r="H33" s="11">
-        <v>0.65727143044199998</v>
-      </c>
-      <c r="I33" s="12">
-        <v>0.657131045887</v>
-      </c>
-      <c r="J33" s="12">
-        <v>0.65720123066699998</v>
-      </c>
-      <c r="K33">
+      <c r="K45" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="L45" s="11">
         <v>0.66928998201400003</v>
       </c>
-      <c r="L33">
+      <c r="M45" s="11">
         <v>0.66914703045299995</v>
       </c>
-      <c r="M33">
+      <c r="N45" s="11">
         <v>0.66921849859899996</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="34">
-        <v>0.57668373429599995</v>
-      </c>
-      <c r="C34" s="34">
-        <v>0.57656056221600005</v>
-      </c>
-      <c r="D34" s="34">
-        <v>0.57662214167799997</v>
-      </c>
-      <c r="E34" s="13">
-        <v>0.59163111867600005</v>
-      </c>
-      <c r="F34" s="14">
-        <v>0.591504754031</v>
-      </c>
-      <c r="G34" s="14">
-        <v>0.59156792960500004</v>
-      </c>
-      <c r="H34" s="13">
-        <v>0.59170003238900004</v>
-      </c>
-      <c r="I34" s="14">
-        <v>0.59157365302499998</v>
-      </c>
-      <c r="J34" s="14">
-        <v>0.59163683595799998</v>
-      </c>
-      <c r="K34">
-        <v>0.62832077955200005</v>
-      </c>
-      <c r="L34">
-        <v>0.62818657847600001</v>
-      </c>
-      <c r="M34">
-        <v>0.62825367184699998</v>
+    <row r="46" spans="1:14">
+      <c r="A46" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="19">
+        <v>0.56646083847899997</v>
+      </c>
+      <c r="C46" s="20">
+        <v>0.56545012165499997</v>
+      </c>
+      <c r="D46" s="24">
+        <v>0.56595502881699999</v>
+      </c>
+      <c r="E46" s="13">
+        <v>0.40314730694399997</v>
+      </c>
+      <c r="F46" s="14">
+        <v>0.40308191403100002</v>
+      </c>
+      <c r="G46" s="52">
+        <v>0.40311460783500003</v>
+      </c>
+      <c r="H46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="L46" s="13">
+        <v>0.67394165765000003</v>
+      </c>
+      <c r="M46" s="14">
+        <v>0.67379771255300003</v>
+      </c>
+      <c r="N46" s="52">
+        <v>0.67386967741500003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="11">
+        <v>0.57751056223599995</v>
+      </c>
+      <c r="C47" s="12">
+        <v>0.57648012976499996</v>
+      </c>
+      <c r="D47" s="23">
+        <v>0.57699488594899995</v>
+      </c>
+      <c r="E47" s="11">
+        <v>0.40898767034400002</v>
+      </c>
+      <c r="F47" s="12">
+        <v>0.408921330089</v>
+      </c>
+      <c r="G47" s="23">
+        <v>0.40895449752599999</v>
+      </c>
+      <c r="K47" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="L47" s="11">
+        <v>0.67556802128100002</v>
+      </c>
+      <c r="M47" s="12">
+        <v>0.67542372881400004</v>
+      </c>
+      <c r="N47" s="23">
+        <v>0.67549586734099998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="13">
+        <v>0.58271043223899999</v>
+      </c>
+      <c r="C48" s="14">
+        <v>0.58167072181699997</v>
+      </c>
+      <c r="D48" s="52">
+        <v>0.58219011283400002</v>
+      </c>
+      <c r="E48" s="13">
+        <v>0.40979883192700001</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.40973236009699998</v>
+      </c>
+      <c r="G48" s="52">
+        <v>0.40976559331700002</v>
+      </c>
+      <c r="K48" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="L48" s="13">
+        <v>0.67829700432100004</v>
+      </c>
+      <c r="M48" s="14">
+        <v>0.67815212897900001</v>
+      </c>
+      <c r="N48" s="52">
+        <v>0.67822455891300004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="53">
+        <v>0.58563535911599995</v>
+      </c>
+      <c r="C49" s="54">
+        <v>0.58459042984599996</v>
+      </c>
+      <c r="D49" s="54">
+        <v>0.58511242795700003</v>
+      </c>
+      <c r="E49" s="53">
+        <v>0.40963659961100002</v>
+      </c>
+      <c r="F49" s="54">
+        <v>0.40957015409600001</v>
+      </c>
+      <c r="G49" s="55">
+        <v>0.40960337415800002</v>
+      </c>
+      <c r="K49" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49" s="53">
+        <v>0.67681535948799998</v>
+      </c>
+      <c r="M49" s="54">
+        <v>0.67667080060600004</v>
+      </c>
+      <c r="N49" s="55">
+        <v>0.67674307232800002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>